<commit_message>
Se agrega set de pruebas
</commit_message>
<xml_diff>
--- a/BugTracker.xlsx
+++ b/BugTracker.xlsx
@@ -1,34 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EA949A71-315B-4412-AFF1-8A68603C6FB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iSony\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{947FF4DD-8134-4A3E-AB70-471251E8CA96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="BugTracker" sheetId="1" r:id="rId1"/>
+    <sheet name="Set de pruebas" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="70">
   <si>
     <t>NRO</t>
   </si>
@@ -109,13 +102,147 @@
   </si>
   <si>
     <t>Medio</t>
+  </si>
+  <si>
+    <t>Nombre del caso</t>
+  </si>
+  <si>
+    <t>Descripcion del caso</t>
+  </si>
+  <si>
+    <t>Pasos</t>
+  </si>
+  <si>
+    <t>Acciones</t>
+  </si>
+  <si>
+    <t>Resultado esperado</t>
+  </si>
+  <si>
+    <t>Aplicaciones</t>
+  </si>
+  <si>
+    <t>Modulo</t>
+  </si>
+  <si>
+    <t>Tipo de prueba</t>
+  </si>
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>CP-001</t>
+  </si>
+  <si>
+    <t>CP-002</t>
+  </si>
+  <si>
+    <t>CP-003</t>
+  </si>
+  <si>
+    <t>CP-004</t>
+  </si>
+  <si>
+    <t>CP-005</t>
+  </si>
+  <si>
+    <t>CP-006</t>
+  </si>
+  <si>
+    <t>El sistema debe mostrar todas las categorias disponibles (Universidad Choucair, Cursos y certificaciones, Seleccion Choucair y Plan carrera)</t>
+  </si>
+  <si>
+    <t>El usuario solo podra ingresar a la categoria de Universidad Choucair si esta matriculado</t>
+  </si>
+  <si>
+    <t>El usuario solo podra ingresar a la categoria de Cursos y Certifaciones si esta matriculado</t>
+  </si>
+  <si>
+    <t>En la categoria de cursos y certificaciones debe mostrar todos los cusos que el usuario puedra realizar</t>
+  </si>
+  <si>
+    <t>En el modulo de cursos y certificaciones se debe mostrar una lista desplegable con las diferentes categorias y cursos.</t>
+  </si>
+  <si>
+    <t>Al momento de ingresar a cualquier curso, si el usuario no esta matriculado, debe aparecer el mensaje de "No se puede auto matricular en este curso"</t>
+  </si>
+  <si>
+    <t>1. Ingresar a la plataforma Choucair Academy.
+2. Ingresar a la categoria de cursos y certificaciones.
+3. Clic em cualquiera de los cursos que aparecen.</t>
+  </si>
+  <si>
+    <t>1. Ingresar a la plataforma Choucair Academy.</t>
+  </si>
+  <si>
+    <t>1. Ingresar a la plataforma Choucair Academy.
+2. Ingresar a la categoria de cursos y certificaciones</t>
+  </si>
+  <si>
+    <t>1. Ingresar a la plataforma Choucair Academy.
+2. Clic en la categoria de cursos y certificaciones.</t>
+  </si>
+  <si>
+    <t>1. Ingresar a la plataforma Choucair Academy.
+2. Ingresar a la categoria Universidad Choucair</t>
+  </si>
+  <si>
+    <t>El sistema debe permitir ingresar al usuario y ver todas la categorias disponibles</t>
+  </si>
+  <si>
+    <t>El sistema no debe permitir ingresar al modulo si no esta matriculado</t>
+  </si>
+  <si>
+    <t>El aplicativo no debe permitir ingresar al modulo si no esta matriculado en ningun curso</t>
+  </si>
+  <si>
+    <t>El sistema debe mostrar un listado con todos los cursos disponibles y que puede realizar el usuario</t>
+  </si>
+  <si>
+    <t>El aplicativo debe mostrar una lista desplegable donde se muestren las escuelas y los cursos disponibles para el usuario</t>
+  </si>
+  <si>
+    <t>Se debe mostrar en pantalla el mensaje "No se puede automatricular en este curso"</t>
+  </si>
+  <si>
+    <t>El usuario ingresara al aplicativo e iniciara sesion</t>
+  </si>
+  <si>
+    <t>El usuario ingresara a la categoria de Universidad Choucair</t>
+  </si>
+  <si>
+    <t>EL usuario ingresara a la categoria Cursos y Certificaciones</t>
+  </si>
+  <si>
+    <t>El sistema debe mostras un mensaje indicando que el usuario no puede auto matricularse</t>
+  </si>
+  <si>
+    <t>Se debe mostrar un listado despues de ingresdar al modulo de Cursos y Certificaciones</t>
+  </si>
+  <si>
+    <t>Se debe ver en pantalla una lista desplegable con todas las escuales y cursos donde puede ingresar el usuario</t>
+  </si>
+  <si>
+    <t>Funcional</t>
+  </si>
+  <si>
+    <t>Choucair Academy</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>Categorias</t>
+  </si>
+  <si>
+    <t>Cursos y certificaciones</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -141,8 +268,22 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -153,6 +294,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF1F497D"/>
         <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -224,7 +371,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -250,6 +397,24 @@
     </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -269,7 +434,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -557,7 +722,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -567,11 +732,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:M6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="0.85546875" customWidth="1"/>
     <col min="3" max="3" width="31.140625" bestFit="1" customWidth="1"/>
@@ -581,8 +746,8 @@
     <col min="12" max="12" width="26.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" ht="4.5" customHeight="1"/>
-    <row r="2" spans="2:13" ht="22.5">
+    <row r="1" spans="2:13" ht="4.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:13" ht="24" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
@@ -620,7 +785,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="2:13" ht="20.25">
+    <row r="3" spans="2:13" ht="22.5" x14ac:dyDescent="0.25">
       <c r="B3" s="1">
         <v>1</v>
       </c>
@@ -638,7 +803,7 @@
       </c>
       <c r="G3" s="3">
         <f ca="1">TODAY()</f>
-        <v>44911</v>
+        <v>44916</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>15</v>
@@ -657,7 +822,7 @@
       </c>
       <c r="M3" s="5"/>
     </row>
-    <row r="4" spans="2:13" ht="20.25">
+    <row r="4" spans="2:13" ht="22.5" x14ac:dyDescent="0.25">
       <c r="B4" s="7">
         <v>2</v>
       </c>
@@ -675,7 +840,7 @@
       </c>
       <c r="G4" s="9">
         <f ca="1">TODAY()</f>
-        <v>44911</v>
+        <v>44916</v>
       </c>
       <c r="H4" s="7" t="s">
         <v>15</v>
@@ -694,7 +859,7 @@
       </c>
       <c r="M4" s="7"/>
     </row>
-    <row r="5" spans="2:13">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>3</v>
       </c>
@@ -712,7 +877,7 @@
       </c>
       <c r="G5" s="3">
         <f ca="1">TODAY()</f>
-        <v>44911</v>
+        <v>44916</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>15</v>
@@ -731,7 +896,7 @@
       </c>
       <c r="M5" s="1"/>
     </row>
-    <row r="6" spans="2:13" ht="20.25">
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>4</v>
       </c>
@@ -749,7 +914,7 @@
       </c>
       <c r="G6" s="3">
         <f ca="1">TODAY()</f>
-        <v>44911</v>
+        <v>44916</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>15</v>
@@ -771,4 +936,236 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4920C92-F7F6-4D13-8FB4-341BA745CE87}">
+  <dimension ref="B1:J8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="0.85546875" customWidth="1"/>
+    <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="54.7109375" customWidth="1"/>
+    <col min="5" max="5" width="35.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:10" ht="4.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B2" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="I2" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="B3" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="G3" s="11">
+        <v>1</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="J3" s="11" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="B4" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="G4" s="11">
+        <v>2</v>
+      </c>
+      <c r="H4" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="I4" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="J4" s="11" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="B5" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="G5" s="11">
+        <v>2</v>
+      </c>
+      <c r="H5" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="I5" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="J5" s="11" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="B6" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="G6" s="11">
+        <v>2</v>
+      </c>
+      <c r="H6" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="I6" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="J6" s="11" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="B7" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="G7" s="11">
+        <v>2</v>
+      </c>
+      <c r="H7" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="I7" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="J7" s="11" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" ht="90" x14ac:dyDescent="0.25">
+      <c r="B8" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="G8" s="11">
+        <v>3</v>
+      </c>
+      <c r="H8" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="I8" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="J8" s="11" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>